<commit_message>
Up to and incl. Data Partition
</commit_message>
<xml_diff>
--- a/DataSets_External/EMOutput/Predictive Models_Metadata.xlsx
+++ b/DataSets_External/EMOutput/Predictive Models_Metadata.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Predictive Models_Metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Predictive_Models_Metadata">Predictive Models_Metadata!$A$1:$D$23</definedName>
+    <definedName name="Predictive_Models_Metadata">Predictive Models_Metadata!$A$1:$D$35</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>NAME</t>
   </si>
@@ -49,73 +49,109 @@
     <t>INTERVAL</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Marital_Status</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Kidhome</t>
+  </si>
+  <si>
+    <t>Teenhome</t>
+  </si>
+  <si>
+    <t>Dt_Customer</t>
+  </si>
+  <si>
+    <t>Recency</t>
+  </si>
+  <si>
+    <t>MntWines</t>
+  </si>
+  <si>
+    <t>MntFruits</t>
+  </si>
+  <si>
+    <t>MntMeatProducts</t>
+  </si>
+  <si>
+    <t>MntFishProducts</t>
+  </si>
+  <si>
+    <t>MntSweetProducts</t>
+  </si>
+  <si>
+    <t>MntGoldProds</t>
+  </si>
+  <si>
+    <t>NumDealsPurchases</t>
+  </si>
+  <si>
+    <t>NumWebPurchases</t>
+  </si>
+  <si>
+    <t>NumCatalogPurchases</t>
+  </si>
+  <si>
+    <t>NumStorePurchases</t>
+  </si>
+  <si>
+    <t>NumWebVisitsMonth</t>
+  </si>
+  <si>
+    <t>AcceptedCmp3</t>
   </si>
   <si>
     <t>BINARY</t>
   </si>
   <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>Marital_Status</t>
-  </si>
-  <si>
-    <t>Dependents</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Dt_Customer</t>
-  </si>
-  <si>
-    <t>Rcn</t>
-  </si>
-  <si>
-    <t>Frq</t>
-  </si>
-  <si>
-    <t>Mnt</t>
-  </si>
-  <si>
-    <t>Clothes</t>
-  </si>
-  <si>
-    <t>Kitchen</t>
-  </si>
-  <si>
-    <t>SmallAppliances</t>
-  </si>
-  <si>
-    <t>HouseKeeping</t>
-  </si>
-  <si>
-    <t>Toys</t>
-  </si>
-  <si>
-    <t>NetPurchase</t>
-  </si>
-  <si>
-    <t>CatPurchase</t>
-  </si>
-  <si>
-    <t>Recomendation</t>
-  </si>
-  <si>
-    <t>CostPerContact</t>
+    <t>AcceptedCmp4</t>
+  </si>
+  <si>
+    <t>AcceptedCmp5</t>
+  </si>
+  <si>
+    <t>AcceptedCmp1</t>
+  </si>
+  <si>
+    <t>AcceptedCmp2</t>
+  </si>
+  <si>
+    <t>Complain</t>
+  </si>
+  <si>
+    <t>Z_CostContact</t>
   </si>
   <si>
     <t>REJECTED</t>
   </si>
   <si>
-    <t>RevenuePerPositiveAnswer</t>
+    <t>Z_Revenue</t>
   </si>
   <si>
     <t>DepVar</t>
   </si>
   <si>
     <t>TARGET</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Element1</t>
+  </si>
+  <si>
+    <t>Element2</t>
+  </si>
+  <si>
+    <t>Element3</t>
+  </si>
+  <si>
+    <t>Element4</t>
   </si>
 </sst>
 </file>
@@ -251,12 +287,12 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -270,7 +306,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -279,12 +315,12 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -293,12 +329,12 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -312,7 +348,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -326,7 +362,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -340,7 +376,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -354,7 +390,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -368,7 +404,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -382,7 +418,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -396,7 +432,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -410,7 +446,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -424,7 +460,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -438,7 +474,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -452,7 +488,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -466,7 +502,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -480,13 +516,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -494,30 +530,198 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
         <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="D23" t="s">
-        <v>11</v>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>